<commit_message>
commit ke3 yg ini dr publik dari cmd, isi file berubah
</commit_message>
<xml_diff>
--- a/undangan.xlsx
+++ b/undangan.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_temp\git_dev\gitgithubdenyoga\publik\publik\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="97">
   <si>
     <t>Nanik Subani, S.Pd.</t>
   </si>
@@ -301,13 +306,19 @@
   </si>
   <si>
     <t>Darso</t>
+  </si>
+  <si>
+    <t>text baru</t>
+  </si>
+  <si>
+    <t>utk ujicoba git</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -352,6 +363,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -398,7 +417,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -430,9 +449,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -464,6 +484,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -639,20 +660,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C58"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27.85546875" customWidth="1"/>
     <col min="3" max="3" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -663,7 +684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -671,7 +692,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -682,7 +703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -693,7 +714,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -704,7 +725,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -715,7 +736,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -726,7 +747,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -734,7 +755,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -745,7 +766,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -756,7 +777,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
@@ -767,7 +788,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
@@ -778,7 +799,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
@@ -789,7 +810,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
@@ -800,7 +821,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
@@ -811,7 +832,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>16</v>
       </c>
@@ -822,7 +843,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>17</v>
       </c>
@@ -833,7 +854,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>18</v>
       </c>
@@ -841,7 +862,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>19</v>
       </c>
@@ -849,7 +870,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20</v>
       </c>
@@ -860,7 +881,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>21</v>
       </c>
@@ -871,7 +892,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>22</v>
       </c>
@@ -882,7 +903,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>23</v>
       </c>
@@ -893,7 +914,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>24</v>
       </c>
@@ -904,7 +925,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>25</v>
       </c>
@@ -915,7 +936,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>26</v>
       </c>
@@ -926,7 +947,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>27</v>
       </c>
@@ -937,7 +958,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>28</v>
       </c>
@@ -948,7 +969,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>29</v>
       </c>
@@ -959,7 +980,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>30</v>
       </c>
@@ -970,7 +991,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>31</v>
       </c>
@@ -981,7 +1002,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>32</v>
       </c>
@@ -992,7 +1013,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>33</v>
       </c>
@@ -1003,7 +1024,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>34</v>
       </c>
@@ -1014,7 +1035,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>35</v>
       </c>
@@ -1025,7 +1046,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>36</v>
       </c>
@@ -1036,7 +1057,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>37</v>
       </c>
@@ -1047,7 +1068,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>38</v>
       </c>
@@ -1058,7 +1079,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>39</v>
       </c>
@@ -1069,7 +1090,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>40</v>
       </c>
@@ -1080,7 +1101,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>41</v>
       </c>
@@ -1091,7 +1112,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>42</v>
       </c>
@@ -1099,7 +1120,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>43</v>
       </c>
@@ -1107,7 +1128,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>44</v>
       </c>
@@ -1115,7 +1136,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>45</v>
       </c>
@@ -1123,7 +1144,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>46</v>
       </c>
@@ -1131,7 +1152,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>47</v>
       </c>
@@ -1142,7 +1163,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>48</v>
       </c>
@@ -1153,7 +1174,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>49</v>
       </c>
@@ -1164,7 +1185,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>50</v>
       </c>
@@ -1175,7 +1196,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>51</v>
       </c>
@@ -1186,7 +1207,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>52</v>
       </c>
@@ -1197,7 +1218,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>53</v>
       </c>
@@ -1205,7 +1226,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>54</v>
       </c>
@@ -1213,7 +1234,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>55</v>
       </c>
@@ -1221,7 +1242,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>56</v>
       </c>
@@ -1229,7 +1250,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>57</v>
       </c>
@@ -1240,9 +1261,17 @@
         <v>93</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>95</v>
+      </c>
+      <c r="C61" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1252,24 +1281,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>